<commit_message>
:sparkles: Pagando informações corretas do cliente
</commit_message>
<xml_diff>
--- a/CalculateClientSecurityHash/Data/Input/ACME-WorkItems.xlsx
+++ b/CalculateClientSecurityHash/Data/Input/ACME-WorkItems.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <x:si>
     <x:t>WIID</x:t>
   </x:si>
@@ -37,16 +37,19 @@
     <x:t>WI5</x:t>
   </x:si>
   <x:si>
+    <x:t>Completed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>87285152</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Research Client Check Copy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>WI2</x:t>
+  </x:si>
+  <x:si>
     <x:t>Open</x:t>
-  </x:si>
-  <x:si>
-    <x:t>87285152</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Research Client Check Copy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>WI2</x:t>
   </x:si>
   <x:si>
     <x:t>87285155</x:t>
@@ -484,12 +487,12 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:4">
       <x:c r="A4" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
         <x:v>9</x:v>
@@ -498,96 +501,96 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
       <x:c r="A5" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:4">
       <x:c r="A6" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4">
       <x:c r="A7" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:4">
       <x:c r="A8" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:4">
       <x:c r="A9" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:4">
       <x:c r="A10" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:4">
       <x:c r="A11" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
         <x:v>5</x:v>

</xml_diff>